<commit_message>
feat: 自动添加每日生成文件 AIPEFinanceDataETF.xlsx (Colab)
</commit_message>
<xml_diff>
--- a/data/AIPEFinanceDataETF.xlsx
+++ b/data/AIPEFinanceDataETF.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,144 +508,148 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>159691</t>
+          <t>513120</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>港股红利ETF</t>
+          <t>港股创新药ETF</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.19</v>
+        <v>1.13</v>
       </c>
       <c r="E2" t="n">
-        <v>1.11</v>
+        <v>4.72</v>
       </c>
       <c r="F2" t="n">
-        <v>6.56</v>
+        <v>56</v>
       </c>
       <c r="G2" t="n">
-        <v>1.48</v>
+        <v>69.95999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>1.171</v>
+        <v>1.073</v>
       </c>
       <c r="I2" t="n">
-        <v>1.1624</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+        <v>1.0308</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.01124999999999987</v>
+      </c>
       <c r="L2" t="b">
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>0.002699999999999925</v>
+        <v>0.01569999999999983</v>
       </c>
       <c r="N2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>512890</t>
+          <t>513060</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>红利低波ETF</t>
+          <t>恒生医疗ETF</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.17</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.26</v>
+        <v>4.07</v>
       </c>
       <c r="F3" t="n">
-        <v>3.91</v>
+        <v>44.1</v>
       </c>
       <c r="G3" t="n">
-        <v>2.66</v>
+        <v>19.76</v>
       </c>
       <c r="H3" t="n">
-        <v>1.165</v>
+        <v>0.538</v>
       </c>
       <c r="I3" t="n">
-        <v>1.1583</v>
+        <v>0.5225000000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>1.15</v>
+        <v>0.504</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002600000000000158</v>
+        <v>0.004100000000000048</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0.001500000000000057</v>
+        <v>0.006000000000000005</v>
       </c>
       <c r="N3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>513120</t>
+          <t>513330</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>港股创新药ETF</t>
+          <t>恒生互联网ETF</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.08</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="n">
-        <v>2.27</v>
+        <v>2.89</v>
       </c>
       <c r="F4" t="n">
-        <v>48.97</v>
+        <v>19.42</v>
       </c>
       <c r="G4" t="n">
-        <v>49.56</v>
+        <v>27.59</v>
       </c>
       <c r="H4" t="n">
-        <v>1.043</v>
+        <v>0.481</v>
       </c>
       <c r="I4" t="n">
-        <v>1.0061</v>
+        <v>0.4753</v>
       </c>
       <c r="J4" t="n">
-        <v>0.956</v>
+        <v>0.478</v>
       </c>
       <c r="K4" t="n">
-        <v>0.009050000000000225</v>
+        <v>0.001299999999999968</v>
       </c>
       <c r="L4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.01029999999999998</v>
+        <v>0.002899999999999958</v>
       </c>
       <c r="N4" t="b">
         <v>0</v>
@@ -654,48 +658,48 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>513060</t>
+          <t>562860</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>恒生医疗ETF</t>
+          <t>生物疫苗ETF</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.54</v>
+        <v>0.67</v>
       </c>
       <c r="E5" t="n">
-        <v>1.69</v>
+        <v>2.61</v>
       </c>
       <c r="F5" t="n">
-        <v>38.46</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="H5" t="n">
-        <v>0.528</v>
+        <v>0.658</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5134000000000001</v>
+        <v>0.6425</v>
       </c>
       <c r="J5" t="n">
-        <v>0.497</v>
+        <v>0.627</v>
       </c>
       <c r="K5" t="n">
-        <v>0.003099999999999936</v>
+        <v>0.003399999999999959</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>0.003300000000000081</v>
+        <v>0.005000000000000004</v>
       </c>
       <c r="N5" t="b">
         <v>0</v>
@@ -704,98 +708,98 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>515880</t>
+          <t>159643</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>通信ETF</t>
+          <t>疫苗ETF</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.3</v>
+        <v>0.59</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6899999999999999</v>
+        <v>1.88</v>
       </c>
       <c r="F6" t="n">
-        <v>-4.33</v>
+        <v>0.51</v>
       </c>
       <c r="G6" t="n">
-        <v>2.8</v>
+        <v>0.08</v>
       </c>
       <c r="H6" t="n">
-        <v>1.254</v>
+        <v>0.588</v>
       </c>
       <c r="I6" t="n">
-        <v>1.2352</v>
+        <v>0.5790999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>1.241</v>
+        <v>0.572</v>
       </c>
       <c r="K6" t="n">
-        <v>0.004699999999999926</v>
+        <v>0.001950000000000007</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>0.006500000000000172</v>
+        <v>0.00219999999999998</v>
       </c>
       <c r="N6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>510410</t>
+          <t>515880</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>资源ETF</t>
+          <t>通信ETF</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.22</v>
+        <v>1.33</v>
       </c>
       <c r="E7" t="n">
-        <v>0.58</v>
+        <v>1.76</v>
       </c>
       <c r="F7" t="n">
-        <v>0.91</v>
+        <v>-2.64</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05</v>
+        <v>2.56</v>
       </c>
       <c r="H7" t="n">
-        <v>1.212</v>
+        <v>1.283</v>
       </c>
       <c r="I7" t="n">
-        <v>1.2116</v>
+        <v>1.2542</v>
       </c>
       <c r="J7" t="n">
-        <v>1.209</v>
+        <v>1.248</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0008000000000001339</v>
+        <v>0.004700000000000149</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0008999999999999009</v>
+        <v>0.01200000000000001</v>
       </c>
       <c r="N7" t="b">
         <v>0</v>
@@ -804,48 +808,48 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>515900</t>
+          <t>159825</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>央企创新驱动ETF</t>
+          <t>农业ETF</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.44</v>
+        <v>0.72</v>
       </c>
       <c r="E8" t="n">
-        <v>0.49</v>
+        <v>1.55</v>
       </c>
       <c r="F8" t="n">
-        <v>-4.65</v>
+        <v>8.41</v>
       </c>
       <c r="G8" t="n">
-        <v>0.14</v>
+        <v>0.72</v>
       </c>
       <c r="H8" t="n">
-        <v>1.424</v>
+        <v>0.712</v>
       </c>
       <c r="I8" t="n">
-        <v>1.4213</v>
+        <v>0.701</v>
       </c>
       <c r="J8" t="n">
-        <v>1.427</v>
+        <v>0.694</v>
       </c>
       <c r="K8" t="n">
-        <v>0.000900000000000345</v>
+        <v>0.001800000000000135</v>
       </c>
       <c r="L8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.000700000000000145</v>
+        <v>0.003599999999999937</v>
       </c>
       <c r="N8" t="b">
         <v>0</v>
@@ -854,48 +858,48 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>512800</t>
+          <t>512170</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>银行ETF</t>
+          <t>医疗ETF</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.64</v>
+        <v>0.34</v>
       </c>
       <c r="E9" t="n">
-        <v>0.31</v>
+        <v>1.52</v>
       </c>
       <c r="F9" t="n">
-        <v>10.3</v>
+        <v>2.45</v>
       </c>
       <c r="G9" t="n">
-        <v>2.87</v>
+        <v>5.89</v>
       </c>
       <c r="H9" t="n">
-        <v>1.629</v>
+        <v>0.334</v>
       </c>
       <c r="I9" t="n">
-        <v>1.6193</v>
+        <v>0.3295</v>
       </c>
       <c r="J9" t="n">
-        <v>1.608</v>
+        <v>0.327</v>
       </c>
       <c r="K9" t="n">
-        <v>0.004899999999999904</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>0.002800000000000358</v>
+        <v>0.001400000000000012</v>
       </c>
       <c r="N9" t="b">
         <v>0</v>
@@ -904,48 +908,48 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>560070</t>
+          <t>513290</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>央企红利ETF基金</t>
+          <t>纳指生物科技ETF</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1.02</v>
+        <v>1.12</v>
       </c>
       <c r="E10" t="n">
-        <v>0.29</v>
+        <v>1.45</v>
       </c>
       <c r="F10" t="n">
-        <v>-3.4</v>
+        <v>-2.94</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01</v>
+        <v>0.42</v>
       </c>
       <c r="H10" t="n">
-        <v>1.024</v>
+        <v>1.105</v>
       </c>
       <c r="I10" t="n">
-        <v>1.0224</v>
+        <v>1.0998</v>
       </c>
       <c r="J10" t="n">
-        <v>1.02</v>
+        <v>1.087</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0009999999999998899</v>
+        <v>0.003000000000000114</v>
       </c>
       <c r="L10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.001300000000000079</v>
+        <v>0.003600000000000048</v>
       </c>
       <c r="N10" t="b">
         <v>0</v>
@@ -954,48 +958,48 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>510760</t>
+          <t>512660</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上证综指ETF</t>
+          <t>军工ETF</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="E11" t="n">
-        <v>0.19</v>
+        <v>1.43</v>
       </c>
       <c r="F11" t="n">
-        <v>2.66</v>
+        <v>1.92</v>
       </c>
       <c r="G11" t="n">
-        <v>0.47</v>
+        <v>6.5</v>
       </c>
       <c r="H11" t="n">
-        <v>1.075</v>
+        <v>1.051</v>
       </c>
       <c r="I11" t="n">
-        <v>1.0711</v>
+        <v>1.0449</v>
       </c>
       <c r="J11" t="n">
-        <v>1.071</v>
+        <v>1.047</v>
       </c>
       <c r="K11" t="n">
-        <v>0.001049999999999995</v>
+        <v>0.0006500000000000394</v>
       </c>
       <c r="L11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.000199999999999978</v>
+        <v>0.003100000000000103</v>
       </c>
       <c r="N11" t="b">
         <v>0</v>
@@ -1004,48 +1008,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>510900</t>
+          <t>512000</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>H股ETF</t>
+          <t>券商ETF</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.11</v>
+        <v>1.03</v>
       </c>
       <c r="E12" t="n">
-        <v>0.18</v>
+        <v>1.37</v>
       </c>
       <c r="F12" t="n">
-        <v>17.37</v>
+        <v>-7.59</v>
       </c>
       <c r="G12" t="n">
-        <v>2.2</v>
+        <v>5.79</v>
       </c>
       <c r="H12" t="n">
-        <v>1.099</v>
+        <v>1.02</v>
       </c>
       <c r="I12" t="n">
-        <v>1.0976</v>
+        <v>1.0084</v>
       </c>
       <c r="J12" t="n">
-        <v>1.098</v>
+        <v>1.015</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00134999999999974</v>
+        <v>0.001500000000000057</v>
       </c>
       <c r="L12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0008000000000001339</v>
+        <v>0.003200000000000092</v>
       </c>
       <c r="N12" t="b">
         <v>0</v>
@@ -1054,98 +1058,98 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>512500</t>
+          <t>512010</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>中证500ETF华夏</t>
+          <t>医药ETF</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.17</v>
+        <v>0.38</v>
       </c>
       <c r="E13" t="n">
-        <v>0.13</v>
+        <v>1.34</v>
       </c>
       <c r="F13" t="n">
-        <v>1.15</v>
+        <v>4.71</v>
       </c>
       <c r="G13" t="n">
-        <v>0.74</v>
+        <v>6.07</v>
       </c>
       <c r="H13" t="n">
-        <v>3.144</v>
+        <v>0.377</v>
       </c>
       <c r="I13" t="n">
-        <v>3.1277</v>
+        <v>0.3727</v>
       </c>
       <c r="J13" t="n">
-        <v>3.141</v>
+        <v>0.369</v>
       </c>
       <c r="K13" t="n">
-        <v>0.001049999999999773</v>
+        <v>0.001099999999999934</v>
       </c>
       <c r="L13" t="b">
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>0.00140000000000029</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="N13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>510210</t>
+          <t>515790</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上证指数ETF</t>
+          <t>光伏ETF</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.84</v>
+        <v>0.66</v>
       </c>
       <c r="E14" t="n">
-        <v>0.12</v>
+        <v>1.24</v>
       </c>
       <c r="F14" t="n">
-        <v>2.94</v>
+        <v>-13.47</v>
       </c>
       <c r="G14" t="n">
-        <v>1.29</v>
+        <v>2.88</v>
       </c>
       <c r="H14" t="n">
-        <v>0.836</v>
+        <v>0.648</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8317</v>
+        <v>0.6468</v>
       </c>
       <c r="J14" t="n">
-        <v>0.829</v>
+        <v>0.658</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001149999999999984</v>
+        <v>4.999999999999449e-05</v>
       </c>
       <c r="L14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.000500000000000056</v>
+        <v>0.0009000000000001229</v>
       </c>
       <c r="N14" t="b">
         <v>0</v>
@@ -1154,48 +1158,48 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>159666</t>
+          <t>159883</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>交通运输ETF</t>
+          <t>医疗器械ETF</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1</v>
+        <v>1.24</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.01</v>
+        <v>1.03</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01</v>
+        <v>0.45</v>
       </c>
       <c r="H15" t="n">
-        <v>0.987</v>
+        <v>0.488</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9847999999999999</v>
+        <v>0.4824</v>
       </c>
       <c r="J15" t="n">
-        <v>0.981</v>
+        <v>0.479</v>
       </c>
       <c r="K15" t="n">
-        <v>0.001049999999999995</v>
+        <v>0.001149999999999984</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.001100000000000101</v>
+        <v>0.001500000000000057</v>
       </c>
       <c r="N15" t="b">
         <v>0</v>
@@ -1204,48 +1208,48 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>513520</t>
+          <t>516670</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>日经ETF</t>
+          <t>畜牧养殖ETF</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.46</v>
+        <v>0.67</v>
       </c>
       <c r="E16" t="n">
-        <v>0.07000000000000001</v>
+        <v>1.21</v>
       </c>
       <c r="F16" t="n">
-        <v>0.21</v>
+        <v>7.57</v>
       </c>
       <c r="G16" t="n">
-        <v>0.48</v>
+        <v>0.23</v>
       </c>
       <c r="H16" t="n">
-        <v>1.462</v>
+        <v>0.666</v>
       </c>
       <c r="I16" t="n">
-        <v>1.4581</v>
+        <v>0.6577</v>
       </c>
       <c r="J16" t="n">
-        <v>1.452</v>
+        <v>0.653</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0009999999999998899</v>
+        <v>0.001399999999999957</v>
       </c>
       <c r="L16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.001300000000000079</v>
+        <v>0.002399999999999847</v>
       </c>
       <c r="N16" t="b">
         <v>0</v>
@@ -1254,48 +1258,48 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>510050</t>
+          <t>510900</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上证50ETF</t>
+          <t>H股ETF</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.76</v>
+        <v>1.13</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07000000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="F17" t="n">
-        <v>0.66</v>
+        <v>18.74</v>
       </c>
       <c r="G17" t="n">
-        <v>13.97</v>
+        <v>3.14</v>
       </c>
       <c r="H17" t="n">
-        <v>2.753</v>
+        <v>1.111</v>
       </c>
       <c r="I17" t="n">
-        <v>2.7598</v>
+        <v>1.1012</v>
       </c>
       <c r="J17" t="n">
-        <v>2.768</v>
+        <v>1.102</v>
       </c>
       <c r="K17" t="n">
-        <v>0.001450000000000173</v>
+        <v>0.002349999999999852</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.003300000000000303</v>
+        <v>0.002599999999999936</v>
       </c>
       <c r="N17" t="b">
         <v>0</v>
@@ -1304,48 +1308,48 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>515080</t>
+          <t>516510</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>中证红利ETF</t>
+          <t>云计算ETF</t>
         </is>
       </c>
       <c r="D18" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="G18" t="n">
         <v>1.53</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-1.34</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.89</v>
-      </c>
       <c r="H18" t="n">
-        <v>1.527</v>
+        <v>1.132</v>
       </c>
       <c r="I18" t="n">
-        <v>1.5249</v>
+        <v>1.1149</v>
       </c>
       <c r="J18" t="n">
-        <v>1.524</v>
+        <v>1.121</v>
       </c>
       <c r="K18" t="n">
-        <v>0.001599999999999824</v>
+        <v>0.0008499999999997954</v>
       </c>
       <c r="L18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.00120000000000009</v>
+        <v>0.007600000000000051</v>
       </c>
       <c r="N18" t="b">
         <v>0</v>
@@ -1354,48 +1358,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>510300</t>
+          <t>515230</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>沪深300ETF</t>
+          <t>软件ETF</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3.99</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05</v>
+        <v>1.12</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.9</v>
+        <v>4.09</v>
       </c>
       <c r="G19" t="n">
-        <v>19.48</v>
+        <v>0.67</v>
       </c>
       <c r="H19" t="n">
-        <v>3.969</v>
+        <v>0.801</v>
       </c>
       <c r="I19" t="n">
-        <v>3.9706</v>
+        <v>0.79</v>
       </c>
       <c r="J19" t="n">
-        <v>3.982</v>
+        <v>0.796</v>
       </c>
       <c r="K19" t="n">
-        <v>0.003150000000000208</v>
+        <v>-0.0001499999999998725</v>
       </c>
       <c r="L19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.002899999999999903</v>
+        <v>0.003700000000000037</v>
       </c>
       <c r="N19" t="b">
         <v>0</v>
@@ -1404,48 +1408,48 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>515800</t>
+          <t>562390</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>800ETF</t>
+          <t>中药50ETF</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.4</v>
+        <v>-0.9</v>
       </c>
       <c r="G20" t="n">
-        <v>0.54</v>
+        <v>0.01</v>
       </c>
       <c r="H20" t="n">
-        <v>1.003</v>
+        <v>0.986</v>
       </c>
       <c r="I20" t="n">
-        <v>1.0018</v>
+        <v>0.9762999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>1.005</v>
+        <v>0.969</v>
       </c>
       <c r="K20" t="n">
-        <v>0.000700000000000145</v>
+        <v>0.002049999999999996</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.0004999999999999449</v>
+        <v>0.00219999999999998</v>
       </c>
       <c r="N20" t="b">
         <v>0</v>
@@ -1454,48 +1458,48 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>562390</t>
+          <t>159949</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>中药50ETF</t>
+          <t>创业板50ETF</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.98</v>
+        <v>0.91</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>-1.9</v>
+        <v>-5.2</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01</v>
+        <v>5.82</v>
       </c>
       <c r="H21" t="n">
-        <v>0.981</v>
+        <v>0.899</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9724</v>
+        <v>0.8919</v>
       </c>
       <c r="J21" t="n">
-        <v>0.965</v>
+        <v>0.901</v>
       </c>
       <c r="K21" t="n">
-        <v>0.00165000000000004</v>
+        <v>0.001049999999999995</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0008000000000001339</v>
+        <v>0.001100000000000101</v>
       </c>
       <c r="N21" t="b">
         <v>0</v>
@@ -1504,48 +1508,48 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>513500</t>
+          <t>159781</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>标普500ETF</t>
+          <t>科创创业ETF</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2.02</v>
+        <v>0.54</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.05</v>
+        <v>0.93</v>
       </c>
       <c r="F22" t="n">
-        <v>-6.38</v>
+        <v>-4.25</v>
       </c>
       <c r="G22" t="n">
-        <v>1.72</v>
+        <v>0.52</v>
       </c>
       <c r="H22" t="n">
-        <v>2.019</v>
+        <v>0.534</v>
       </c>
       <c r="I22" t="n">
-        <v>2.007</v>
+        <v>0.5291</v>
       </c>
       <c r="J22" t="n">
-        <v>1.998</v>
+        <v>0.532</v>
       </c>
       <c r="K22" t="n">
-        <v>0.004900000000000349</v>
+        <v>0.0003999999999999559</v>
       </c>
       <c r="L22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0009999999999998899</v>
+        <v>0.001199999999999979</v>
       </c>
       <c r="N22" t="b">
         <v>0</v>
@@ -1554,48 +1558,48 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>513800</t>
+          <t>512980</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>日本东证指数ETF</t>
+          <t>传媒ETF</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1.47</v>
+        <v>0.83</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.2</v>
+        <v>0.85</v>
       </c>
       <c r="F23" t="n">
-        <v>7.75</v>
+        <v>6.72</v>
       </c>
       <c r="G23" t="n">
-        <v>0.06</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H23" t="n">
-        <v>1.484</v>
+        <v>0.82</v>
       </c>
       <c r="I23" t="n">
-        <v>1.4782</v>
+        <v>0.8101</v>
       </c>
       <c r="J23" t="n">
-        <v>1.465</v>
+        <v>0.805</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0006999999999999229</v>
+        <v>0.001449999999999951</v>
       </c>
       <c r="L23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>0.00120000000000009</v>
+        <v>0.004200000000000093</v>
       </c>
       <c r="N23" t="b">
         <v>0</v>
@@ -1604,48 +1608,48 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>510230</t>
+          <t>159915</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>金融ETF</t>
+          <t>创业板ETF</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1.37</v>
+        <v>2.03</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.22</v>
+        <v>0.84</v>
       </c>
       <c r="F24" t="n">
-        <v>4.9</v>
+        <v>-3.24</v>
       </c>
       <c r="G24" t="n">
-        <v>0.23</v>
+        <v>17.22</v>
       </c>
       <c r="H24" t="n">
-        <v>1.36</v>
+        <v>2.009</v>
       </c>
       <c r="I24" t="n">
-        <v>1.3542</v>
+        <v>1.9911</v>
       </c>
       <c r="J24" t="n">
-        <v>1.351</v>
+        <v>2.006</v>
       </c>
       <c r="K24" t="n">
-        <v>0.003350000000000186</v>
+        <v>0.002299999999999969</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>0.001400000000000068</v>
+        <v>0.003600000000000048</v>
       </c>
       <c r="N24" t="b">
         <v>0</v>
@@ -1654,48 +1658,48 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>513100</t>
+          <t>159667</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>纳指ETF</t>
+          <t>工业母机ETF</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.57</v>
+        <v>1.12</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.25</v>
+        <v>0.63</v>
       </c>
       <c r="F25" t="n">
-        <v>-3.81</v>
+        <v>11.18</v>
       </c>
       <c r="G25" t="n">
-        <v>6.06</v>
+        <v>0.31</v>
       </c>
       <c r="H25" t="n">
-        <v>1.57</v>
+        <v>1.111</v>
       </c>
       <c r="I25" t="n">
-        <v>1.5586</v>
+        <v>1.107</v>
       </c>
       <c r="J25" t="n">
-        <v>1.547</v>
+        <v>1.121</v>
       </c>
       <c r="K25" t="n">
-        <v>0.005400000000000071</v>
+        <v>0</v>
       </c>
       <c r="L25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>0.002099999999999991</v>
+        <v>0.001100000000000101</v>
       </c>
       <c r="N25" t="b">
         <v>0</v>
@@ -1704,48 +1708,48 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>159915</t>
+          <t>512500</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>创业板ETF</t>
+          <t>中证500ETF华夏</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2.02</v>
+        <v>3.19</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.3</v>
+        <v>0.63</v>
       </c>
       <c r="F26" t="n">
-        <v>-4.04</v>
+        <v>1.78</v>
       </c>
       <c r="G26" t="n">
-        <v>10.38</v>
+        <v>2.04</v>
       </c>
       <c r="H26" t="n">
-        <v>1.992</v>
+        <v>3.164</v>
       </c>
       <c r="I26" t="n">
-        <v>1.9871</v>
+        <v>3.1406</v>
       </c>
       <c r="J26" t="n">
-        <v>2.003</v>
+        <v>3.144</v>
       </c>
       <c r="K26" t="n">
-        <v>0.002650000000000485</v>
+        <v>0.002450000000000063</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.001399999999999846</v>
+        <v>0.008399999999999963</v>
       </c>
       <c r="N26" t="b">
         <v>0</v>
@@ -1754,48 +1758,48 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>159652</t>
+          <t>513520</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>有色50ETF</t>
+          <t>日经ETF</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.93</v>
+        <v>1.47</v>
       </c>
       <c r="E27" t="n">
-        <v>0.86</v>
+        <v>0.62</v>
       </c>
       <c r="F27" t="n">
-        <v>9.5</v>
+        <v>0.83</v>
       </c>
       <c r="G27" t="n">
-        <v>0.11</v>
+        <v>0.74</v>
       </c>
       <c r="H27" t="n">
-        <v>0.919</v>
+        <v>1.46</v>
       </c>
       <c r="I27" t="n">
-        <v>0.9201</v>
+        <v>1.4622</v>
       </c>
       <c r="J27" t="n">
-        <v>0.92</v>
+        <v>1.453</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0004499999999998394</v>
+        <v>0.0009999999999998899</v>
       </c>
       <c r="L27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.0008000000000001339</v>
+        <v>0.002799999999999914</v>
       </c>
       <c r="N27" t="b">
         <v>0</v>
@@ -1804,48 +1808,48 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>159825</t>
+          <t>516010</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>农业ETF</t>
+          <t>游戏ETF</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.71</v>
+        <v>1.16</v>
       </c>
       <c r="E28" t="n">
-        <v>0.71</v>
+        <v>0.61</v>
       </c>
       <c r="F28" t="n">
-        <v>6.76</v>
+        <v>16.35</v>
       </c>
       <c r="G28" t="n">
-        <v>0.63</v>
+        <v>0.97</v>
       </c>
       <c r="H28" t="n">
-        <v>0.705</v>
+        <v>1.151</v>
       </c>
       <c r="I28" t="n">
-        <v>0.6955</v>
+        <v>1.1292</v>
       </c>
       <c r="J28" t="n">
-        <v>0.6909999999999999</v>
+        <v>1.108</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0009999999999998899</v>
+        <v>0.003550000000000164</v>
       </c>
       <c r="L28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" t="n">
-        <v>0.001700000000000035</v>
+        <v>0.008000000000000007</v>
       </c>
       <c r="N28" t="b">
         <v>0</v>
@@ -1854,48 +1858,48 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>516020</t>
+          <t>515210</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>化工ETF</t>
+          <t>钢铁ETF</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.6</v>
+        <v>1.21</v>
       </c>
       <c r="E29" t="n">
-        <v>0.68</v>
+        <v>0.58</v>
       </c>
       <c r="F29" t="n">
-        <v>-1.81</v>
+        <v>2.72</v>
       </c>
       <c r="G29" t="n">
-        <v>0.08</v>
+        <v>0.79</v>
       </c>
       <c r="H29" t="n">
-        <v>0.59</v>
+        <v>1.198</v>
       </c>
       <c r="I29" t="n">
-        <v>0.5891999999999999</v>
+        <v>1.2013</v>
       </c>
       <c r="J29" t="n">
-        <v>0.593</v>
+        <v>1.214</v>
       </c>
       <c r="K29" t="n">
-        <v>0.000199999999999978</v>
+        <v>-0.0006500000000000394</v>
       </c>
       <c r="L29" t="b">
         <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>9.999999999998899e-05</v>
+        <v>-0.000199999999999978</v>
       </c>
       <c r="N29" t="b">
         <v>0</v>
@@ -1904,48 +1908,48 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>513330</t>
+          <t>159770</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>恒生互联网ETF</t>
+          <t>机器人ETF</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.48</v>
+        <v>0.88</v>
       </c>
       <c r="E30" t="n">
-        <v>0.62</v>
+        <v>0.57</v>
       </c>
       <c r="F30" t="n">
-        <v>16.07</v>
+        <v>8.56</v>
       </c>
       <c r="G30" t="n">
-        <v>15.09</v>
+        <v>1.42</v>
       </c>
       <c r="H30" t="n">
-        <v>0.473</v>
+        <v>0.869</v>
       </c>
       <c r="I30" t="n">
-        <v>0.4712</v>
+        <v>0.8689</v>
       </c>
       <c r="J30" t="n">
-        <v>0.476</v>
+        <v>0.886</v>
       </c>
       <c r="K30" t="n">
-        <v>-4.999999999993898e-05</v>
+        <v>-0.001050000000000106</v>
       </c>
       <c r="L30" t="b">
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.0003000000000000225</v>
+        <v>0.000299999999999967</v>
       </c>
       <c r="N30" t="b">
         <v>0</v>
@@ -1954,48 +1958,48 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>513290</t>
+          <t>588000</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>纳指生物科技ETF</t>
+          <t>科创50ETF</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.11</v>
+        <v>1.05</v>
       </c>
       <c r="E31" t="n">
-        <v>0.55</v>
+        <v>0.57</v>
       </c>
       <c r="F31" t="n">
-        <v>-4.33</v>
+        <v>0.77</v>
       </c>
       <c r="G31" t="n">
-        <v>0.37</v>
+        <v>17.28</v>
       </c>
       <c r="H31" t="n">
-        <v>1.101</v>
+        <v>1.044</v>
       </c>
       <c r="I31" t="n">
-        <v>1.0958</v>
+        <v>1.0378</v>
       </c>
       <c r="J31" t="n">
-        <v>1.082</v>
+        <v>1.043</v>
       </c>
       <c r="K31" t="n">
-        <v>0.002299999999999969</v>
+        <v>-0.000299999999999967</v>
       </c>
       <c r="L31" t="b">
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>0.000700000000000145</v>
+        <v>0.002000000000000224</v>
       </c>
       <c r="N31" t="b">
         <v>0</v>
@@ -2004,48 +2008,48 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>515220</t>
+          <t>513500</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>煤炭ETF</t>
+          <t>标普500ETF</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.99</v>
+        <v>2.04</v>
       </c>
       <c r="E32" t="n">
-        <v>0.41</v>
+        <v>0.54</v>
       </c>
       <c r="F32" t="n">
-        <v>-12.89</v>
+        <v>-5.87</v>
       </c>
       <c r="G32" t="n">
-        <v>1.86</v>
+        <v>1.96</v>
       </c>
       <c r="H32" t="n">
-        <v>0.987</v>
+        <v>2.026</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9885999999999999</v>
+        <v>2.0164</v>
       </c>
       <c r="J32" t="n">
-        <v>0.987</v>
+        <v>2.007</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0007999999999999119</v>
+        <v>0.004900000000000126</v>
       </c>
       <c r="L32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.002000000000000002</v>
+        <v>0.005399999999999849</v>
       </c>
       <c r="N32" t="b">
         <v>0</v>
@@ -2054,48 +2058,48 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>561560</t>
+          <t>510230</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>电力ETF</t>
+          <t>金融ETF</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.17</v>
+        <v>1.38</v>
       </c>
       <c r="E33" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5.43</v>
+      </c>
+      <c r="G33" t="n">
         <v>0.34</v>
       </c>
-      <c r="F33" t="n">
-        <v>-2.25</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.43</v>
-      </c>
       <c r="H33" t="n">
-        <v>1.174</v>
+        <v>1.372</v>
       </c>
       <c r="I33" t="n">
-        <v>1.1775</v>
+        <v>1.3588</v>
       </c>
       <c r="J33" t="n">
-        <v>1.178</v>
+        <v>1.357</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0002499999999998614</v>
+        <v>0.002699999999999925</v>
       </c>
       <c r="L33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.002500000000000169</v>
+        <v>0.003299999999999859</v>
       </c>
       <c r="N33" t="b">
         <v>0</v>
@@ -2104,48 +2108,48 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>516510</t>
+          <t>515070</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>云计算ETF</t>
+          <t>人工智能AIETF</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.15</v>
+        <v>1.19</v>
       </c>
       <c r="E34" t="n">
-        <v>0.26</v>
+        <v>0.51</v>
       </c>
       <c r="F34" t="n">
-        <v>3.99</v>
+        <v>2.84</v>
       </c>
       <c r="G34" t="n">
-        <v>1.75</v>
+        <v>1.03</v>
       </c>
       <c r="H34" t="n">
-        <v>1.114</v>
+        <v>1.173</v>
       </c>
       <c r="I34" t="n">
-        <v>1.1036</v>
+        <v>1.1585</v>
       </c>
       <c r="J34" t="n">
-        <v>1.121</v>
+        <v>1.166</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.0001500000000000945</v>
+        <v>0.0004500000000000615</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.003600000000000048</v>
+        <v>0.004199999999999982</v>
       </c>
       <c r="N34" t="b">
         <v>0</v>
@@ -2154,48 +2158,48 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>511090</t>
+          <t>516020</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>30年国债ETF</t>
+          <t>化工ETF</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>123.34</v>
+        <v>0.6</v>
       </c>
       <c r="E35" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5600000000000001</v>
+        <v>-1.32</v>
       </c>
       <c r="G35" t="n">
-        <v>55.76</v>
+        <v>0.08</v>
       </c>
       <c r="H35" t="n">
-        <v>122.97</v>
+        <v>0.593</v>
       </c>
       <c r="I35" t="n">
-        <v>123.0676</v>
+        <v>0.5898</v>
       </c>
       <c r="J35" t="n">
-        <v>123.29</v>
+        <v>0.593</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.03829999999997824</v>
+        <v>0.0004499999999998394</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.0002000000000066393</v>
+        <v>0.001000000000000001</v>
       </c>
       <c r="N35" t="b">
         <v>0</v>
@@ -2204,48 +2208,48 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>515070</t>
+          <t>159928</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>人工智能AIETF</t>
+          <t>消费ETF</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.19</v>
+        <v>0.82</v>
       </c>
       <c r="E36" t="n">
-        <v>0.17</v>
+        <v>0.49</v>
       </c>
       <c r="F36" t="n">
-        <v>2.33</v>
+        <v>0.73</v>
       </c>
       <c r="G36" t="n">
-        <v>1.43</v>
+        <v>2.89</v>
       </c>
       <c r="H36" t="n">
-        <v>1.158</v>
+        <v>0.821</v>
       </c>
       <c r="I36" t="n">
-        <v>1.1526</v>
+        <v>0.8198000000000001</v>
       </c>
       <c r="J36" t="n">
-        <v>1.167</v>
+        <v>0.822</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0001500000000000945</v>
+        <v>-0.0001500000000000945</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.002099999999999991</v>
+        <v>0.000200000000000089</v>
       </c>
       <c r="N36" t="b">
         <v>0</v>
@@ -2254,48 +2258,48 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>516670</t>
+          <t>513800</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>畜牧养殖ETF</t>
+          <t>日本东证指数ETF</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.66</v>
+        <v>1.48</v>
       </c>
       <c r="E37" t="n">
-        <v>0.15</v>
+        <v>0.48</v>
       </c>
       <c r="F37" t="n">
-        <v>6.28</v>
+        <v>8.27</v>
       </c>
       <c r="G37" t="n">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="H37" t="n">
-        <v>0.661</v>
+        <v>1.481</v>
       </c>
       <c r="I37" t="n">
-        <v>0.6545</v>
+        <v>1.4819</v>
       </c>
       <c r="J37" t="n">
-        <v>0.651</v>
+        <v>1.468</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0007500000000000284</v>
+        <v>0.001149999999999984</v>
       </c>
       <c r="L37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>0.000299999999999967</v>
+        <v>0.001500000000000057</v>
       </c>
       <c r="N37" t="b">
         <v>0</v>
@@ -2304,48 +2308,48 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>515210</t>
+          <t>515260</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>钢铁ETF</t>
+          <t>电子ETF</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.2</v>
+        <v>0.86</v>
       </c>
       <c r="E38" t="n">
-        <v>0.08</v>
+        <v>0.47</v>
       </c>
       <c r="F38" t="n">
-        <v>2.13</v>
+        <v>-5.07</v>
       </c>
       <c r="G38" t="n">
-        <v>0.47</v>
+        <v>0.09</v>
       </c>
       <c r="H38" t="n">
-        <v>1.198</v>
+        <v>0.85</v>
       </c>
       <c r="I38" t="n">
-        <v>1.2034</v>
+        <v>0.8427999999999999</v>
       </c>
       <c r="J38" t="n">
-        <v>1.216</v>
+        <v>0.849</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.001800000000000024</v>
+        <v>0.0001499999999998725</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>-0.002800000000000136</v>
+        <v>0.00219999999999998</v>
       </c>
       <c r="N38" t="b">
         <v>0</v>
@@ -2354,48 +2358,48 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>512480</t>
+          <t>515220</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>半导体ETF</t>
+          <t>煤炭ETF</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.03</v>
+        <v>0.99</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.41</v>
       </c>
       <c r="F39" t="n">
-        <v>1.78</v>
+        <v>-12.53</v>
       </c>
       <c r="G39" t="n">
-        <v>6.81</v>
+        <v>1.27</v>
       </c>
       <c r="H39" t="n">
-        <v>1.01</v>
+        <v>0.986</v>
       </c>
       <c r="I39" t="n">
-        <v>1.007</v>
+        <v>0.9861000000000001</v>
       </c>
       <c r="J39" t="n">
-        <v>1.023</v>
+        <v>0.988</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.002099999999999769</v>
+        <v>0.0009499999999998954</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0007999999999999119</v>
+        <v>-0.0002999999999998559</v>
       </c>
       <c r="N39" t="b">
         <v>0</v>
@@ -2404,48 +2408,48 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>512200</t>
+          <t>515800</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>房地产ETF</t>
+          <t>800ETF</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1.35</v>
+        <v>1.01</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F40" t="n">
-        <v>-7.32</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0.91</v>
+        <v>2</v>
       </c>
       <c r="H40" t="n">
-        <v>1.347</v>
+        <v>1.006</v>
       </c>
       <c r="I40" t="n">
-        <v>1.3413</v>
+        <v>1.0018</v>
       </c>
       <c r="J40" t="n">
-        <v>1.354</v>
+        <v>1.006</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.001849999999999907</v>
+        <v>0.0005999999999999339</v>
       </c>
       <c r="L40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.001300000000000079</v>
+        <v>0.0005999999999999339</v>
       </c>
       <c r="N40" t="b">
         <v>0</v>
@@ -2454,48 +2458,48 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>512760</t>
+          <t>511090</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>芯片ETF</t>
+          <t>30年国债ETF</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.14</v>
+        <v>123.8</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F41" t="n">
-        <v>1.07</v>
+        <v>0.93</v>
       </c>
       <c r="G41" t="n">
-        <v>2.09</v>
+        <v>67.87</v>
       </c>
       <c r="H41" t="n">
-        <v>1.119</v>
+        <v>123.299</v>
       </c>
       <c r="I41" t="n">
-        <v>1.1168</v>
+        <v>123.1011</v>
       </c>
       <c r="J41" t="n">
-        <v>1.134</v>
+        <v>123.198</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.002399999999999736</v>
+        <v>-0.03024999999998101</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>0.000700000000000145</v>
+        <v>0.04959999999999809</v>
       </c>
       <c r="N41" t="b">
         <v>0</v>
@@ -2504,48 +2508,48 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>518880</t>
+          <t>510760</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>黄金ETF</t>
+          <t>上证综指ETF</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.48</v>
+        <v>1.08</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.03</v>
+        <v>0.37</v>
       </c>
       <c r="F42" t="n">
-        <v>26.2</v>
+        <v>3.04</v>
       </c>
       <c r="G42" t="n">
-        <v>28.08</v>
+        <v>0.57</v>
       </c>
       <c r="H42" t="n">
-        <v>7.42</v>
+        <v>1.078</v>
       </c>
       <c r="I42" t="n">
-        <v>7.4171</v>
+        <v>1.0726</v>
       </c>
       <c r="J42" t="n">
-        <v>7.368</v>
+        <v>1.073</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.009549999999999947</v>
+        <v>0.001049999999999995</v>
       </c>
       <c r="L42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>0.004100000000000215</v>
+        <v>0.001199999999999868</v>
       </c>
       <c r="N42" t="b">
         <v>0</v>
@@ -2554,48 +2558,48 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>159928</t>
+          <t>510210</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>消费ETF</t>
+          <t>上证指数ETF</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.12</v>
+        <v>0.36</v>
       </c>
       <c r="F43" t="n">
-        <v>0.24</v>
+        <v>3.3</v>
       </c>
       <c r="G43" t="n">
-        <v>2.82</v>
+        <v>1.48</v>
       </c>
       <c r="H43" t="n">
-        <v>0.821</v>
+        <v>0.839</v>
       </c>
       <c r="I43" t="n">
-        <v>0.8199</v>
+        <v>0.8333999999999999</v>
       </c>
       <c r="J43" t="n">
-        <v>0.822</v>
+        <v>0.831</v>
       </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>0.001249999999999862</v>
       </c>
       <c r="L43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" t="n">
-        <v>-0.0005999999999998229</v>
+        <v>0.001099999999999879</v>
       </c>
       <c r="N43" t="b">
         <v>0</v>
@@ -2604,48 +2608,48 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>512690</t>
+          <t>512800</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>酒ETF</t>
+          <t>银行ETF</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.58</v>
+        <v>1.64</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.17</v>
+        <v>0.31</v>
       </c>
       <c r="F44" t="n">
-        <v>-6.33</v>
+        <v>10.64</v>
       </c>
       <c r="G44" t="n">
-        <v>4.58</v>
+        <v>4.86</v>
       </c>
       <c r="H44" t="n">
-        <v>0.58</v>
+        <v>1.64</v>
       </c>
       <c r="I44" t="n">
-        <v>0.5832999999999999</v>
+        <v>1.6228</v>
       </c>
       <c r="J44" t="n">
-        <v>0.592</v>
+        <v>1.615</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.0009500000000000064</v>
+        <v>0.003150000000000208</v>
       </c>
       <c r="L44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" t="n">
-        <v>-0.001400000000000068</v>
+        <v>0.003000000000000114</v>
       </c>
       <c r="N44" t="b">
         <v>0</v>
@@ -2654,48 +2658,48 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>159781</t>
+          <t>512200</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>科创创业ETF</t>
+          <t>房地产ETF</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.54</v>
+        <v>1.36</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.19</v>
+        <v>0.3</v>
       </c>
       <c r="F45" t="n">
-        <v>-5.13</v>
+        <v>-7.05</v>
       </c>
       <c r="G45" t="n">
-        <v>0.25</v>
+        <v>1.06</v>
       </c>
       <c r="H45" t="n">
-        <v>0.53</v>
+        <v>1.353</v>
       </c>
       <c r="I45" t="n">
-        <v>0.5279</v>
+        <v>1.3457</v>
       </c>
       <c r="J45" t="n">
-        <v>0.532</v>
+        <v>1.353</v>
       </c>
       <c r="K45" t="n">
-        <v>0.0004499999999999504</v>
+        <v>-4.999999999988347e-05</v>
       </c>
       <c r="L45" t="b">
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0003999999999999559</v>
+        <v>0.002999999999999892</v>
       </c>
       <c r="N45" t="b">
         <v>0</v>
@@ -2704,48 +2708,48 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>515260</t>
+          <t>513100</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>电子ETF</t>
+          <t>纳指ETF</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.86</v>
+        <v>1.57</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.23</v>
+        <v>0.26</v>
       </c>
       <c r="F46" t="n">
-        <v>-5.51</v>
+        <v>-3.56</v>
       </c>
       <c r="G46" t="n">
-        <v>0.06</v>
+        <v>3.46</v>
       </c>
       <c r="H46" t="n">
-        <v>0.841</v>
+        <v>1.569</v>
       </c>
       <c r="I46" t="n">
-        <v>0.8398</v>
+        <v>1.5651</v>
       </c>
       <c r="J46" t="n">
-        <v>0.85</v>
+        <v>1.555</v>
       </c>
       <c r="K46" t="n">
-        <v>-0.000500000000000167</v>
+        <v>0.004199999999999982</v>
       </c>
       <c r="L46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>0.001000000000000001</v>
+        <v>0.003599999999999826</v>
       </c>
       <c r="N46" t="b">
         <v>0</v>
@@ -2754,48 +2758,48 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>515790</t>
+          <t>510300</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>光伏ETF</t>
+          <t>沪深300ETF</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.65</v>
+        <v>4</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.31</v>
+        <v>0.23</v>
       </c>
       <c r="F47" t="n">
-        <v>-14.53</v>
+        <v>-0.67</v>
       </c>
       <c r="G47" t="n">
-        <v>1.35</v>
+        <v>23.23</v>
       </c>
       <c r="H47" t="n">
-        <v>0.644</v>
+        <v>3.98</v>
       </c>
       <c r="I47" t="n">
-        <v>0.6472</v>
+        <v>3.9681</v>
       </c>
       <c r="J47" t="n">
-        <v>0.659</v>
+        <v>3.986</v>
       </c>
       <c r="K47" t="n">
-        <v>-0.0003999999999999559</v>
+        <v>0.002749999999999364</v>
       </c>
       <c r="L47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" t="n">
-        <v>-0.001599999999999935</v>
+        <v>0.001199999999999424</v>
       </c>
       <c r="N47" t="b">
         <v>0</v>
@@ -2804,48 +2808,48 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>159637</t>
+          <t>159652</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>新能源车龙头ETF</t>
+          <t>有色50ETF</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.6</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.33</v>
+        <v>0.21</v>
       </c>
       <c r="F48" t="n">
-        <v>1.69</v>
+        <v>9.73</v>
       </c>
       <c r="G48" t="n">
-        <v>0.05</v>
+        <v>0.16</v>
       </c>
       <c r="H48" t="n">
-        <v>0.598</v>
+        <v>0.93</v>
       </c>
       <c r="I48" t="n">
-        <v>0.6042</v>
+        <v>0.9215</v>
       </c>
       <c r="J48" t="n">
-        <v>0.611</v>
+        <v>0.922</v>
       </c>
       <c r="K48" t="n">
-        <v>-9.999999999998899e-05</v>
+        <v>0.001450000000000173</v>
       </c>
       <c r="L48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" t="n">
-        <v>-0.003199999999999981</v>
+        <v>0.001099999999999879</v>
       </c>
       <c r="N48" t="b">
         <v>0</v>
@@ -2854,50 +2858,400 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>588000</t>
+          <t>512480</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-09</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>科创50ETF</t>
+          <t>半导体ETF</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.38</v>
+        <v>0.19</v>
       </c>
       <c r="F49" t="n">
-        <v>0.19</v>
+        <v>1.98</v>
       </c>
       <c r="G49" t="n">
-        <v>15.71</v>
+        <v>6.19</v>
       </c>
       <c r="H49" t="n">
-        <v>1.039</v>
+        <v>1.019</v>
       </c>
       <c r="I49" t="n">
-        <v>1.0349</v>
+        <v>1.0103</v>
       </c>
       <c r="J49" t="n">
-        <v>1.045</v>
+        <v>1.02</v>
       </c>
       <c r="K49" t="n">
-        <v>-0.00154999999999994</v>
+        <v>-0.0006500000000000394</v>
       </c>
       <c r="L49" t="b">
         <v>0</v>
       </c>
       <c r="M49" t="n">
-        <v>0.0004999999999999449</v>
+        <v>0.002599999999999936</v>
       </c>
       <c r="N49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>515080</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>中证红利ETF</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-1.21</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1.528</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1.5237</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1.526</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.001049999999999995</v>
+      </c>
+      <c r="L50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.000299999999999967</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>515250</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>智能汽车ETF</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.9488999999999999</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="K51" t="n">
+        <v>-0.0003500000000000725</v>
+      </c>
+      <c r="L51" t="b">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>-0.000100000000000211</v>
+      </c>
+      <c r="N51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>561560</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>电力ETF</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-2.17</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1.1751</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1.178</v>
+      </c>
+      <c r="K52" t="n">
+        <v>-0.0002499999999998614</v>
+      </c>
+      <c r="L52" t="b">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>-0.0004999999999999449</v>
+      </c>
+      <c r="N52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>512890</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>红利低波ETF</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F53" t="n">
+        <v>4</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1.1607</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1.154</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.001900000000000013</v>
+      </c>
+      <c r="L53" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.00199999999999978</v>
+      </c>
+      <c r="N53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>515900</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>央企创新驱动ETF</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-4.58</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1.423</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1.428</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.0008500000000000174</v>
+      </c>
+      <c r="L54" t="b">
+        <v>1</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.00240000000000018</v>
+      </c>
+      <c r="N54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>512760</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>芯片ETF</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1.1195</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1.131</v>
+      </c>
+      <c r="K55" t="n">
+        <v>-0.0007999999999999119</v>
+      </c>
+      <c r="L55" t="b">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.002399999999999958</v>
+      </c>
+      <c r="N55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>159637</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>新能源车龙头ETF</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.599</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.6001</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="K56" t="n">
+        <v>-0.0003499999999999615</v>
+      </c>
+      <c r="L56" t="b">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>-0.002000000000000002</v>
+      </c>
+      <c r="N56" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>